<commit_message>
Journal de bord Alexandre
</commit_message>
<xml_diff>
--- a/Journaux de bord/JournalDeBord-AlexandreGratton.xlsx
+++ b/Journaux de bord/JournalDeBord-AlexandreGratton.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,16 @@
     <t>Création procédures stockées
 Aide au GUI
 Conception base de donnée</t>
+  </si>
+  <si>
+    <t>mercredi 2 février 2016</t>
+  </si>
+  <si>
+    <t>Création procédure stockée
+GUI
+Tests sur la bd
+Ajout création de compte
+Ajout checkbox dynamiques GUI</t>
   </si>
 </sst>
 </file>
@@ -83,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -134,11 +144,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,6 +191,12 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1048556"/>
+  <dimension ref="A1:B1048557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,44 +547,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="5" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="6" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1048556" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1048556" s="2"/>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1048557" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>